<commit_message>
Update to print status
</commit_message>
<xml_diff>
--- a/Star Trek Ship Prints.xlsx
+++ b/Star Trek Ship Prints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\EAGLE\projects\DS9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F912E996-2E4B-49E3-8FC6-5D656A020388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DE59E2-8454-4658-A1C2-7739660E612F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9765" yWindow="840" windowWidth="19305" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29325" yWindow="1650" windowWidth="32205" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ships" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="118">
   <si>
     <t>Length (m)</t>
   </si>
@@ -509,7 +509,7 @@
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -517,6 +517,14 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -800,7 +808,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,85 +867,100 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1451.82</v>
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>170</v>
       </c>
       <c r="C2" s="3">
-        <f>(B2/$J$1)*1000</f>
-        <v>439.94545454545454</v>
+        <f t="shared" ref="C2:C33" si="0">(B2/$J$1)*1000</f>
+        <v>51.515151515151516</v>
       </c>
       <c r="D2" s="3">
-        <f>C2/10*0.393701</f>
-        <v>17.32069654</v>
+        <f t="shared" ref="D2:D33" si="1">C2/10*0.393701</f>
+        <v>2.0281566666666668</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>170</v>
+        <v>243</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C56" si="0">(B3/$J$1)*1000</f>
-        <v>51.515151515151516</v>
+        <f t="shared" si="0"/>
+        <v>73.63636363636364</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D56" si="1">C3/10*0.393701</f>
-        <v>2.0281566666666668</v>
-      </c>
-      <c r="E3" t="s">
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>2.8990710000000002</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L3" t="s">
         <v>86</v>
       </c>
       <c r="M3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
+      <c r="A4" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>305</v>
+        <v>467</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" si="0"/>
-        <v>92.424242424242422</v>
+        <v>141.5151515151515</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="1"/>
-        <v>3.6387516666666668</v>
+        <v>5.5714656666666666</v>
+      </c>
+      <c r="F4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" t="s">
+        <v>111</v>
+      </c>
+      <c r="O4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>23.1</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>243</v>
-      </c>
-      <c r="C5" s="3">
-        <f t="shared" si="0"/>
-        <v>73.63636363636364</v>
-      </c>
       <c r="D5" s="3">
         <f t="shared" si="1"/>
-        <v>2.8990710000000002</v>
+        <v>0.27559070000000002</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L5" t="s">
         <v>86</v>
@@ -951,21 +974,21 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>467</v>
+        <v>371.88</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>141.5151515151515</v>
+        <v>112.69090909090909</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="1"/>
-        <v>5.5714656666666666</v>
+        <v>4.4366523600000001</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>101</v>
@@ -976,138 +999,169 @@
       <c r="N6" t="s">
         <v>111</v>
       </c>
+      <c r="O6" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
+      <c r="A7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>641</v>
+        <v>245</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="0"/>
-        <v>194.24242424242425</v>
+        <v>74.242424242424249</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="1"/>
-        <v>7.6473436666666679</v>
+        <v>2.9229316666666669</v>
+      </c>
+      <c r="F7" t="s">
+        <v>102</v>
+      </c>
+      <c r="M7" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
+      <c r="A8" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B8">
-        <v>231</v>
+        <v>150.81</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>45.699999999999996</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="1"/>
-        <v>2.7559070000000001</v>
+        <v>1.7992135699999998</v>
+      </c>
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+      <c r="M8" t="s">
+        <v>111</v>
       </c>
       <c r="N8" s="9" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>11</v>
+      <c r="A9" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="B9">
-        <v>535.20000000000005</v>
+        <v>85.78</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="0"/>
-        <v>162.18181818181822</v>
+        <v>25.993939393939396</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="1"/>
-        <v>6.3851144000000017</v>
+        <v>1.0233839933333335</v>
+      </c>
+      <c r="O9" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>12</v>
+      <c r="A10" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B10">
-        <v>685</v>
+        <v>157.76</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="0"/>
-        <v>207.57575757575759</v>
+        <v>47.806060606060605</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="1"/>
-        <v>8.1722783333333346</v>
+        <v>1.8821293866666666</v>
+      </c>
+      <c r="F10" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B11">
-        <v>23.1</v>
+        <v>150</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>45.454545454545453</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="1"/>
-        <v>0.27559070000000002</v>
-      </c>
-      <c r="F11" t="s">
-        <v>97</v>
-      </c>
+        <v>1.78955</v>
+      </c>
+      <c r="F11" s="6"/>
       <c r="L11" s="9" t="s">
         <v>105</v>
       </c>
+      <c r="M11" t="s">
+        <v>111</v>
+      </c>
+      <c r="O11" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>14</v>
+      <c r="A12" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B12">
-        <v>442.23</v>
+        <v>270</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="0"/>
-        <v>134.0090909090909</v>
+        <v>81.818181818181813</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="1"/>
-        <v>5.2759513099999999</v>
-      </c>
-      <c r="E12" t="s">
-        <v>108</v>
+        <v>3.22119</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="M12" t="s">
+        <v>111</v>
       </c>
       <c r="N12" s="9" t="s">
         <v>101</v>
       </c>
+      <c r="O12" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="B13">
-        <v>371.88</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="0"/>
-        <v>112.69090909090909</v>
+        <v>6.3636363636363642</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>4.4366523600000001</v>
+        <v>0.25053700000000007</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>86</v>
@@ -1118,159 +1172,165 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="B14">
-        <v>245</v>
+        <v>255.65</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="0"/>
-        <v>74.242424242424249</v>
+        <v>77.469696969696969</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="1"/>
-        <v>2.9229316666666669</v>
-      </c>
-      <c r="F14" t="s">
-        <v>102</v>
-      </c>
+        <v>3.049989716666667</v>
+      </c>
+      <c r="F14" s="6"/>
       <c r="L14" s="9" t="s">
         <v>86</v>
       </c>
+      <c r="M14" t="s">
+        <v>111</v>
+      </c>
       <c r="N14" t="s">
         <v>111</v>
       </c>
+      <c r="O14" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>265</v>
+      <c r="A15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="5">
+        <v>235</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="0"/>
-        <v>80.303030303030312</v>
+        <v>71.212121212121218</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="1"/>
-        <v>3.161538333333334</v>
+        <v>2.8036283333333336</v>
+      </c>
+      <c r="F15" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>388</v>
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1451.82</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="0"/>
-        <v>117.57575757575756</v>
+        <v>439.94545454545454</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="1"/>
-        <v>4.628969333333333</v>
+        <v>17.32069654</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>682.32</v>
+        <v>305</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="0"/>
-        <v>206.76363636363638</v>
+        <v>92.424242424242422</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="1"/>
-        <v>8.1403050400000012</v>
+        <v>3.6387516666666668</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>20</v>
+      <c r="A18" t="s">
+        <v>9</v>
       </c>
       <c r="B18">
-        <v>255.65</v>
+        <v>641</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="0"/>
-        <v>77.469696969696969</v>
+        <v>194.24242424242425</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" si="1"/>
-        <v>3.049989716666667</v>
-      </c>
-      <c r="F18" s="6"/>
+        <v>7.6473436666666679</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B19">
-        <v>1041.6500000000001</v>
+        <v>231</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="0"/>
-        <v>315.65151515151518</v>
+        <v>70</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="1"/>
-        <v>12.42723171666667</v>
+        <v>2.7559070000000001</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
+      <c r="A20" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B20">
-        <v>600</v>
+        <v>535.20000000000005</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="0"/>
-        <v>181.81818181818181</v>
+        <v>162.18181818181822</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" si="1"/>
-        <v>7.1581999999999999</v>
+        <v>6.3851144000000017</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
+      <c r="A21" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B21">
-        <v>1282</v>
+        <v>685</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="0"/>
-        <v>388.4848484848485</v>
+        <v>207.57575757575759</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="1"/>
-        <v>15.294687333333336</v>
+        <v>8.1722783333333346</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>24</v>
+      <c r="A22" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B22">
-        <v>388</v>
+        <v>442.23</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="0"/>
-        <v>117.57575757575756</v>
+        <v>134.0090909090909</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="1"/>
-        <v>4.628969333333333</v>
+        <v>5.2759513099999999</v>
       </c>
       <c r="E22" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F22" t="s">
         <v>96</v>
@@ -1284,37 +1344,34 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B23">
-        <v>481.32</v>
+        <v>265</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="0"/>
-        <v>145.85454545454547</v>
+        <v>80.303030303030312</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" si="1"/>
-        <v>5.7423080400000011</v>
+        <v>3.161538333333334</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>26</v>
+      <c r="A24" t="s">
+        <v>18</v>
       </c>
       <c r="B24">
-        <v>150.81</v>
+        <v>388</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="0"/>
-        <v>45.699999999999996</v>
+        <v>117.57575757575756</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" si="1"/>
-        <v>1.7992135699999998</v>
-      </c>
-      <c r="F24" t="s">
-        <v>99</v>
+        <v>4.628969333333333</v>
       </c>
       <c r="L24" s="9" t="s">
         <v>105</v>
@@ -1327,37 +1384,37 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>28</v>
+      <c r="A25" t="s">
+        <v>19</v>
       </c>
       <c r="B25">
-        <v>371.88</v>
+        <v>682.32</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="0"/>
-        <v>112.69090909090909</v>
+        <v>206.76363636363638</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" si="1"/>
-        <v>4.4366523600000001</v>
-      </c>
-      <c r="F25" s="6"/>
+        <v>8.1403050400000012</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>29</v>
+      <c r="A26" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B26">
-        <v>85.78</v>
+        <v>255.65</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="0"/>
-        <v>25.993939393939396</v>
+        <v>77.469696969696969</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="1"/>
-        <v>1.0233839933333335</v>
-      </c>
+        <v>3.049989716666667</v>
+      </c>
+      <c r="F26" s="6"/>
       <c r="L26" s="9" t="s">
         <v>105</v>
       </c>
@@ -1369,21 +1426,20 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>30</v>
+      <c r="A27" t="s">
+        <v>21</v>
       </c>
       <c r="B27">
-        <v>344</v>
+        <v>1041.6500000000001</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="0"/>
-        <v>104.24242424242425</v>
+        <v>315.65151515151518</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" si="1"/>
-        <v>4.1040346666666672</v>
-      </c>
-      <c r="F27" s="9"/>
+        <v>12.42723171666667</v>
+      </c>
       <c r="L27" t="s">
         <v>107</v>
       </c>
@@ -1392,35 +1448,35 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>31</v>
+      <c r="A28" t="s">
+        <v>22</v>
       </c>
       <c r="B28">
-        <v>526</v>
+        <v>600</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="0"/>
-        <v>159.39393939393941</v>
+        <v>181.81818181818181</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" si="1"/>
-        <v>6.2753553333333345</v>
+        <v>7.1581999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B29">
-        <v>221.74</v>
+        <v>1282</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="0"/>
-        <v>67.193939393939402</v>
+        <v>388.4848484848485</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" si="1"/>
-        <v>2.6454321133333338</v>
+        <v>15.294687333333336</v>
       </c>
       <c r="L29" s="9" t="s">
         <v>101</v>
@@ -1430,75 +1486,79 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>33</v>
+      <c r="A30" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B30">
-        <v>487</v>
+        <v>388</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="0"/>
-        <v>147.57575757575759</v>
+        <v>117.57575757575756</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" si="1"/>
-        <v>5.8100723333333342</v>
+        <v>4.628969333333333</v>
+      </c>
+      <c r="E30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>37</v>
+      <c r="A31" t="s">
+        <v>25</v>
       </c>
       <c r="B31">
-        <v>678.36</v>
+        <v>481.32</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="0"/>
-        <v>205.56363636363636</v>
+        <v>145.85454545454547</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" si="1"/>
-        <v>8.0930609199999992</v>
+        <v>5.7423080400000011</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B32">
-        <v>157.76</v>
+        <v>371.88</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="0"/>
-        <v>47.806060606060605</v>
+        <v>112.69090909090909</v>
       </c>
       <c r="D32" s="3">
         <f t="shared" si="1"/>
-        <v>1.8821293866666666</v>
-      </c>
-      <c r="F32" t="s">
-        <v>98</v>
-      </c>
+        <v>4.4366523600000001</v>
+      </c>
+      <c r="F32" s="6"/>
       <c r="N32" s="9" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B33">
-        <v>150</v>
+        <v>344</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" si="0"/>
-        <v>45.454545454545453</v>
+        <v>104.24242424242425</v>
       </c>
       <c r="D33" s="3">
         <f t="shared" si="1"/>
-        <v>1.78955</v>
-      </c>
-      <c r="F33" s="6"/>
+        <v>4.1040346666666672</v>
+      </c>
+      <c r="F33" s="9"/>
       <c r="L33" s="9" t="s">
         <v>106</v>
       </c>
@@ -1507,22 +1567,19 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>36</v>
+      <c r="A34" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="B34">
-        <v>270</v>
+        <v>526</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" si="0"/>
-        <v>81.818181818181813</v>
+        <f t="shared" ref="C34:C65" si="2">(B34/$J$1)*1000</f>
+        <v>159.39393939393941</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" si="1"/>
-        <v>3.22119</v>
-      </c>
-      <c r="F34" t="s">
-        <v>94</v>
+        <f t="shared" ref="D34:D65" si="3">C34/10*0.393701</f>
+        <v>6.2753553333333345</v>
       </c>
       <c r="L34" t="s">
         <v>86</v>
@@ -1535,21 +1592,20 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>103</v>
+      <c r="A35" t="s">
+        <v>32</v>
       </c>
       <c r="B35">
-        <v>255.65</v>
+        <v>221.74</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="0"/>
-        <v>77.469696969696969</v>
+        <f t="shared" si="2"/>
+        <v>67.193939393939402</v>
       </c>
       <c r="D35" s="3">
-        <f t="shared" si="1"/>
-        <v>3.049989716666667</v>
-      </c>
-      <c r="F35" s="6"/>
+        <f t="shared" si="3"/>
+        <v>2.6454321133333338</v>
+      </c>
       <c r="L35" s="9" t="s">
         <v>86</v>
       </c>
@@ -1559,57 +1615,51 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>487</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="2"/>
+        <v>147.57575757575759</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="3"/>
+        <v>5.8100723333333342</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>678.36</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="2"/>
+        <v>205.56363636363636</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="3"/>
+        <v>8.0930609199999992</v>
+      </c>
+      <c r="L37" s="9"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>104</v>
       </c>
-      <c r="B36">
+      <c r="B38">
         <v>33.1</v>
       </c>
-      <c r="C36" s="3">
-        <f t="shared" si="0"/>
+      <c r="C38" s="3">
+        <f t="shared" si="2"/>
         <v>10.030303030303029</v>
       </c>
-      <c r="D36" s="3">
-        <f t="shared" si="1"/>
+      <c r="D38" s="3">
+        <f t="shared" si="3"/>
         <v>0.39489403333333334</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37">
-        <v>3.6</v>
-      </c>
-      <c r="C37" s="3">
-        <f t="shared" si="0"/>
-        <v>1.0909090909090911</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="1"/>
-        <v>4.2949200000000007E-2</v>
-      </c>
-      <c r="E37" t="s">
-        <v>91</v>
-      </c>
-      <c r="L37" s="9"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="5">
-        <v>235</v>
-      </c>
-      <c r="C38" s="3">
-        <f t="shared" si="0"/>
-        <v>71.212121212121218</v>
-      </c>
-      <c r="D38" s="3">
-        <f t="shared" si="1"/>
-        <v>2.8036283333333336</v>
-      </c>
-      <c r="F38" t="s">
-        <v>94</v>
       </c>
       <c r="L38" s="9" t="s">
         <v>105</v>
@@ -1620,18 +1670,21 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="B39">
-        <v>481.32</v>
+        <v>3.6</v>
       </c>
       <c r="C39" s="3">
-        <f t="shared" si="0"/>
-        <v>145.85454545454547</v>
+        <f t="shared" si="2"/>
+        <v>1.0909090909090911</v>
       </c>
       <c r="D39" s="3">
-        <f t="shared" si="1"/>
-        <v>5.7423080400000011</v>
+        <f t="shared" si="3"/>
+        <v>4.2949200000000007E-2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>91</v>
       </c>
       <c r="N39" s="9" t="s">
         <v>101</v>
@@ -1639,59 +1692,53 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40">
+        <v>481.32</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="2"/>
+        <v>145.85454545454547</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="3"/>
+        <v>5.7423080400000011</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>68</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>3037</v>
       </c>
-      <c r="C40" s="3">
-        <f t="shared" si="0"/>
+      <c r="C41" s="3">
+        <f t="shared" si="2"/>
         <v>920.30303030303025</v>
       </c>
-      <c r="D40" s="3">
-        <f t="shared" si="1"/>
+      <c r="D41" s="3">
+        <f t="shared" si="3"/>
         <v>36.232422333333339</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41">
-        <v>24.23</v>
-      </c>
-      <c r="C41" s="3">
-        <f t="shared" si="0"/>
-        <v>7.3424242424242427</v>
-      </c>
-      <c r="D41" s="3">
-        <f t="shared" si="1"/>
-        <v>0.28907197666666667</v>
-      </c>
-      <c r="F41" t="s">
-        <v>97</v>
       </c>
       <c r="L41" s="9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>89</v>
+      <c r="A42" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="B42">
-        <v>21</v>
+        <v>24.23</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="0"/>
-        <v>6.3636363636363642</v>
+        <f t="shared" si="2"/>
+        <v>7.3424242424242427</v>
       </c>
       <c r="D42" s="3">
-        <f t="shared" si="1"/>
-        <v>0.25053700000000007</v>
-      </c>
-      <c r="E42" t="s">
-        <v>90</v>
+        <f t="shared" si="3"/>
+        <v>0.28907197666666667</v>
       </c>
       <c r="F42" t="s">
         <v>97</v>
@@ -1708,11 +1755,11 @@
         <v>90</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>27.27272727272727</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0737300000000001</v>
       </c>
       <c r="F43" s="6"/>
@@ -1731,11 +1778,11 @@
         <v>639.75</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>193.86363636363637</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.6324307500000002</v>
       </c>
     </row>
@@ -1747,11 +1794,11 @@
         <v>68.5</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20.757575757575754</v>
       </c>
       <c r="D45" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.81722783333333315</v>
       </c>
     </row>
@@ -1763,11 +1810,11 @@
         <v>3810</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1154.5454545454545</v>
       </c>
       <c r="D46" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45.454570000000004</v>
       </c>
       <c r="E46" t="s">
@@ -1776,105 +1823,108 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C47" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D47" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C48" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D48" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D49" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D51" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D53" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D54" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D55" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D56" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F56">
+    <sortCondition sortBy="cellColor" ref="A2:A56" dxfId="1"/>
+  </sortState>
   <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>6</formula>

</xml_diff>